<commit_message>
inicio funcionalidades endpoint inventario
</commit_message>
<xml_diff>
--- a/modelando los datos.xlsx
+++ b/modelando los datos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HELMER\2021\gessys-servidor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HELMER\Proyectos\gessys-servidor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53131941-00A2-484C-BD7B-0D18A2E8F324}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12330"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Usuario de Windows</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -132,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -157,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -207,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -232,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -257,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0" shapeId="0">
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -282,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0">
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -307,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0">
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -339,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>MARCA</t>
   </si>
@@ -486,12 +487,15 @@
   </si>
   <si>
     <t>Crear el modelo con un campo tipo array relacionado a coleccion de uevos campos</t>
+  </si>
+  <si>
+    <t>FECHA FACTURA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -593,18 +597,9 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -619,6 +614,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,11 +903,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:T30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C3:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,151 +918,157 @@
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="16.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" customWidth="1"/>
-    <col min="19" max="19" width="22.7109375" customWidth="1"/>
+    <col min="12" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="20" max="20" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-    </row>
-    <row r="5" spans="3:20" ht="90" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+    </row>
+    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+    </row>
+    <row r="5" spans="3:21" ht="90" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="P5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="Q5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="R5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="10" t="s">
+      <c r="S5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="T5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="U5" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>6</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5" t="s">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5" t="s">
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1075,8 +1085,9 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1093,8 +1104,9 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1111,8 +1123,9 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1129,8 +1142,9 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1147,8 +1161,9 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1165,8 +1180,9 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1183,8 +1199,9 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1201,8 +1218,9 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1219,8 +1237,9 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-    </row>
-    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1237,8 +1256,9 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1255,8 +1275,9 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1273,8 +1294,9 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1291,8 +1313,9 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1309,8 +1332,9 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1327,8 +1351,9 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1345,8 +1370,9 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1363,8 +1389,9 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1381,8 +1408,9 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-    </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1399,8 +1427,9 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-    </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1417,8 +1446,9 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-    </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1435,8 +1465,9 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
-    </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="1"/>
+    </row>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1453,8 +1484,9 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
-    </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S28" s="1"/>
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1471,8 +1503,9 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
-    </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1489,10 +1522,11 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C3:R4"/>
+    <mergeCell ref="C3:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1501,7 +1535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1516,154 +1550,154 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="12"/>
+      <c r="G2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="K2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>1</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <v>1</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>2</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <v>2</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>3</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>3</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>2</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>3</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="5">
         <v>4</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="5">
         <v>2</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="6" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
creado modelo de inventario
</commit_message>
<xml_diff>
--- a/modelando los datos.xlsx
+++ b/modelando los datos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HELMER\Proyectos\gessys-servidor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HELMER\2021\gessys-servidor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53131941-00A2-484C-BD7B-0D18A2E8F324}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Usuario de Windows</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -133,32 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Usuario de Windows:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-CAMPO DE TEXTO STRING
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -183,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -208,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -258,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="P5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -283,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="Q5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -308,7 +282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="R5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -340,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>MARCA</t>
   </si>
@@ -355,9 +329,6 @@
   </si>
   <si>
     <t>ASIGNADO</t>
-  </si>
-  <si>
-    <t>RESPONSIBLE</t>
   </si>
   <si>
     <t>PISO</t>
@@ -495,7 +466,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -903,30 +874,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:U30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="16.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="20" max="20" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="16.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -943,9 +913,8 @@
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-    </row>
-    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -962,9 +931,8 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-    </row>
-    <row r="5" spans="3:21" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="3:20" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -981,94 +949,88 @@
         <v>5</v>
       </c>
       <c r="H5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>7</v>
-      </c>
       <c r="K5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="Q5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="R5" s="7" t="s">
+      <c r="S5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="3">
+        <v>6</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="H6" s="3">
-        <v>6</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="N6" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="O6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1085,9 +1047,8 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1104,9 +1065,8 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1123,9 +1083,8 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1142,9 +1101,8 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1161,9 +1119,8 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-    </row>
-    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1180,9 +1137,8 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-    </row>
-    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1199,9 +1155,8 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-    </row>
-    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1218,9 +1173,8 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-    </row>
-    <row r="15" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1237,9 +1191,8 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-    </row>
-    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1256,9 +1209,8 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1275,9 +1227,8 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-    </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1294,9 +1245,8 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-    </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1313,9 +1263,8 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-    </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1332,9 +1281,8 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-    </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1351,9 +1299,8 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-    </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1370,9 +1317,8 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1389,9 +1335,8 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1408,9 +1353,8 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1427,9 +1371,8 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1446,9 +1389,8 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-    </row>
-    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1465,9 +1407,8 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-    </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1484,9 +1425,8 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-    </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1503,9 +1443,8 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-    </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1522,11 +1461,10 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C3:S4"/>
+    <mergeCell ref="C3:R4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1535,7 +1473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1551,50 +1489,50 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="12"/>
       <c r="D2" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
       <c r="K2" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1602,13 +1540,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -1617,13 +1555,13 @@
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1631,13 +1569,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="3">
         <v>2</v>
@@ -1646,13 +1584,13 @@
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="3">
         <v>2</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1660,13 +1598,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>3</v>
@@ -1675,13 +1613,13 @@
         <v>2</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" s="3">
         <v>3</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1689,7 +1627,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="5">
         <v>4</v>
@@ -1698,7 +1636,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
iniciando modelo de crear registro de inventario
</commit_message>
<xml_diff>
--- a/modelando los datos.xlsx
+++ b/modelando los datos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HELMER\2021\gessys-servidor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HELMER\Proyectos\gessys-servidor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA6DAEC-FF36-468D-8429-988DFD9A811E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,12 +26,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Usuario de Windows</author>
+    <author>HELMER VILLARREAL</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -132,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -157,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -178,11 +180,11 @@
           </rPr>
           <t xml:space="preserve">
 DEPENDENCIA QUE REALIZA REGISTRO. 
-SELECTOR.</t>
+SELECTOR. SE DEBE MOSTRAR AL USUARIO SOLO LA CATEGORIA, LA DEPENDENCIA SE CAPTURA DEL LOGIN</t>
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -207,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -232,7 +234,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0" shapeId="0">
+    <comment ref="P5" authorId="1" shapeId="0" xr:uid="{C303D0A7-12C7-49CF-AA5B-969E375CBC76}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>HELMER VILLARREAL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Usuario al que se le asigna el equipo o accesorio, se debe mostrar en el selector solo los usuario de la tabla usuario
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -257,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0">
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -282,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0">
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -314,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>MARCA</t>
   </si>
@@ -457,17 +484,35 @@
     <t>agregar campo de identificacion y tipo al modelo usuarios</t>
   </si>
   <si>
-    <t>Crear el modelo con un campo tipo array relacionado a coleccion de uevos campos</t>
-  </si>
-  <si>
     <t>FECHA FACTURA</t>
+  </si>
+  <si>
+    <t>Crear el modelo con un campo tipo array relacionado a coleccion de nuevos campos</t>
+  </si>
+  <si>
+    <t>RESPONABLE</t>
+  </si>
+  <si>
+    <t>HELMER</t>
+  </si>
+  <si>
+    <t>OSWALDO</t>
+  </si>
+  <si>
+    <t>DAVID</t>
+  </si>
+  <si>
+    <t>USUARIOS</t>
+  </si>
+  <si>
+    <t>Se debe tener en cuenta para futuros registros de equipos, los campos nuevos agregados.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,16 +554,36 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -550,22 +615,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -580,12 +634,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,6 +643,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,11 +940,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:T30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C3:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,53 +952,58 @@
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="17" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="16.28515625" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" customWidth="1"/>
     <col min="15" max="15" width="17.140625" customWidth="1"/>
-    <col min="19" max="19" width="22.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="20" max="20" width="22.7109375" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="10" t="s">
+    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-    </row>
-    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-    </row>
-    <row r="5" spans="3:20" ht="90" x14ac:dyDescent="0.25">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="3:22" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -948,13 +1019,13 @@
       <c r="G5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -964,31 +1035,37 @@
         <v>45</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="S5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="T5" s="9" t="s">
+      <c r="T5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V5" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1004,13 +1081,13 @@
       <c r="G6" s="3">
         <v>6</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="14" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="3" t="s">
@@ -1018,26 +1095,29 @@
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="14" t="s">
         <v>38</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="3" t="s">
+      <c r="R6" s="3"/>
+      <c r="S6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1047,15 +1127,16 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="16"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1065,15 +1146,16 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="16"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1083,15 +1165,16 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="16"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1101,15 +1184,16 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1119,15 +1203,16 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="I12" s="18"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1137,15 +1222,16 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="I13" s="16"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1155,15 +1241,16 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1173,15 +1260,16 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1191,15 +1279,16 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
-    </row>
-    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="16"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1209,15 +1298,16 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="I17" s="16"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1227,15 +1317,16 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="I18" s="16"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1245,15 +1336,16 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="I19" s="16"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1263,15 +1355,16 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="I20" s="16"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1281,15 +1374,16 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="I21" s="16"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1299,15 +1393,16 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="I22" s="16"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1317,15 +1412,16 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="I23" s="16"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1335,15 +1431,16 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="I24" s="16"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1353,15 +1450,16 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-    </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="I25" s="16"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1371,15 +1469,16 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-    </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="I26" s="16"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1389,15 +1488,16 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-    </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="I27" s="16"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1407,15 +1507,16 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
-    </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="1"/>
+    </row>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="I28" s="16"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1425,15 +1526,16 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
-    </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S28" s="1"/>
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="I29" s="16"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1443,15 +1545,16 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
-    </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="I30" s="16"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1461,10 +1564,11 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C3:R4"/>
+    <mergeCell ref="C3:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1473,11 +1577,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,26 +1591,30 @@
     <col min="9" max="9" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="G2" s="12" t="s">
+      <c r="E2" s="10"/>
+      <c r="G2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="K2" s="12" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="K2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" s="10"/>
+      <c r="N2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="10"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1534,8 +1642,14 @@
       <c r="L3" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1563,8 +1677,14 @@
       <c r="L4" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1592,8 +1712,14 @@
       <c r="L5" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="3">
+        <v>2</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1621,8 +1747,14 @@
       <c r="L6" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="3">
+        <v>3</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7" s="5">
         <v>4</v>
       </c>
@@ -1640,11 +1772,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
creando modelo de proveedores, endpoint de crear y traer proveedores y endpoint de crear y traer registros de inventario
</commit_message>
<xml_diff>
--- a/modelando los datos.xlsx
+++ b/modelando los datos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HELMER\Proyectos\gessys-servidor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HELMER\2021\gessys-servidor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA6DAEC-FF36-468D-8429-988DFD9A811E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,13 +25,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Usuario de Windows</author>
     <author>HELMER VILLARREAL</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -134,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -234,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="1" shapeId="0" xr:uid="{C303D0A7-12C7-49CF-AA5B-969E375CBC76}">
+    <comment ref="P5" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="Q5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="R5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -309,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="S5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -511,7 +510,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -634,15 +633,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -661,6 +651,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,11 +939,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +951,7 @@
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="14" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="16.28515625" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" customWidth="1"/>
@@ -964,44 +963,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
     </row>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
     </row>
     <row r="5" spans="3:22" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
@@ -1019,13 +1018,13 @@
       <c r="G5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="10" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -1037,7 +1036,7 @@
       <c r="M5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="O5" s="7" t="s">
@@ -1055,13 +1054,13 @@
       <c r="S5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="T5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="U5" s="12" t="s">
+      <c r="U5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="V5" s="11" t="s">
+      <c r="V5" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1081,13 +1080,13 @@
       <c r="G6" s="3">
         <v>6</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="11" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="11" t="s">
         <v>23</v>
       </c>
       <c r="K6" s="3" t="s">
@@ -1095,7 +1094,7 @@
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="11" t="s">
         <v>38</v>
       </c>
       <c r="O6" s="3" t="s">
@@ -1117,7 +1116,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="16"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1136,7 +1135,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="16"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1155,7 +1154,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="16"/>
+      <c r="I9" s="13"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1174,7 +1173,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="16"/>
+      <c r="I10" s="13"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1193,7 +1192,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="16"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1212,7 +1211,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="18"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1231,7 +1230,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="16"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1250,7 +1249,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="16"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1269,7 +1268,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="16"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1288,7 +1287,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="16"/>
+      <c r="I16" s="13"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1307,7 +1306,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="16"/>
+      <c r="I17" s="13"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1326,7 +1325,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="16"/>
+      <c r="I18" s="13"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1345,7 +1344,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="16"/>
+      <c r="I19" s="13"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1364,7 +1363,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="16"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1383,7 +1382,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="16"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1402,7 +1401,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="16"/>
+      <c r="I22" s="13"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1421,7 +1420,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="16"/>
+      <c r="I23" s="13"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1440,7 +1439,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="16"/>
+      <c r="I24" s="13"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1459,7 +1458,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="16"/>
+      <c r="I25" s="13"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1478,7 +1477,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="16"/>
+      <c r="I26" s="13"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1497,7 +1496,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="16"/>
+      <c r="I27" s="13"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1516,7 +1515,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="16"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1535,7 +1534,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="16"/>
+      <c r="I29" s="13"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1554,7 +1553,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="16"/>
+      <c r="I30" s="13"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1577,7 +1576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1592,27 +1591,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="18"/>
+      <c r="D2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="G2" s="10" t="s">
+      <c r="E2" s="18"/>
+      <c r="G2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="K2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="N2" s="10" t="s">
+      <c r="L2" s="18"/>
+      <c r="N2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="10"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">

</xml_diff>

<commit_message>
Creando endpoint de modificar y eliminar registro de inventario y agregando propiedad campos nuevos
</commit_message>
<xml_diff>
--- a/modelando los datos.xlsx
+++ b/modelando los datos.xlsx
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>MARCA</t>
   </si>
@@ -505,6 +505,9 @@
   </si>
   <si>
     <t>Se debe tener en cuenta para futuros registros de equipos, los campos nuevos agregados.</t>
+  </si>
+  <si>
+    <t>Usuario especial puede modificar solo los campos(anexo, estado, imagenes, responsible, observacion y piso)</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -659,6 +662,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:V30"/>
+  <dimension ref="C3:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,9 +966,10 @@
     <col min="20" max="20" width="22.7109375" customWidth="1"/>
     <col min="21" max="21" width="16.85546875" customWidth="1"/>
     <col min="22" max="22" width="15.5703125" customWidth="1"/>
+    <col min="23" max="23" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
@@ -983,7 +990,7 @@
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
     </row>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -1002,7 +1009,7 @@
       <c r="R4" s="17"/>
       <c r="S4" s="17"/>
     </row>
-    <row r="5" spans="3:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:23" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1063,8 +1070,11 @@
       <c r="V5" s="8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="W5" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1109,7 +1119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1128,7 +1138,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1147,7 +1157,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1166,7 +1176,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1185,7 +1195,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1204,7 +1214,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1223,7 +1233,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1242,7 +1252,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1261,7 +1271,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1280,7 +1290,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>

</xml_diff>

<commit_message>
ajusted modelo inventario y creacion de modelo, route y controller de NuevosCampos
</commit_message>
<xml_diff>
--- a/modelando los datos.xlsx
+++ b/modelando los datos.xlsx
@@ -330,6 +330,7 @@
           <t xml:space="preserve">
 POR ASIGNAR
 ASIGNADO
+GARANTIA
 DADO DE BAJA
 MANTENIMIENTO</t>
         </r>
@@ -340,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>MARCA</t>
   </si>
@@ -508,6 +509,12 @@
   </si>
   <si>
     <t>Usuario especial puede modificar solo los campos(anexo, estado, imagenes, responsible, observacion y piso)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campos que puede modificar usuario especial </t>
+  </si>
+  <si>
+    <t>Info que se captura desde el backend</t>
   </si>
 </sst>
 </file>
@@ -565,7 +572,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +588,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -654,6 +667,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,9 +679,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:W30"/>
+  <dimension ref="C3:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,44 +991,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
     </row>
     <row r="4" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
     </row>
     <row r="5" spans="3:23" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
@@ -1022,7 +1043,7 @@
       <c r="F5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="20" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="10" t="s">
@@ -1037,7 +1058,7 @@
       <c r="K5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="20" t="s">
         <v>45</v>
       </c>
       <c r="M5" s="7" t="s">
@@ -1046,19 +1067,19 @@
       <c r="N5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="R5" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="T5" s="8" t="s">
@@ -1070,7 +1091,7 @@
       <c r="V5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="W5" s="19" t="s">
+      <c r="W5" s="16" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1087,7 +1108,7 @@
       <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="21">
         <v>6</v>
       </c>
       <c r="H6" s="11" t="s">
@@ -1115,7 +1136,7 @@
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="21" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1574,6 +1595,18 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C32" s="22"/>
+      <c r="D32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="23"/>
+      <c r="D33" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1601,27 +1634,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="D2" s="18" t="s">
+      <c r="B2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="G2" s="18" t="s">
+      <c r="E2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="K2" s="18" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="K2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="18"/>
-      <c r="N2" s="18" t="s">
+      <c r="L2" s="19"/>
+      <c r="N2" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="18"/>
+      <c r="O2" s="19"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">

</xml_diff>

<commit_message>
ajuste endpoint crear inventario, valor campos nuevos para almacenarlos
</commit_message>
<xml_diff>
--- a/modelando los datos.xlsx
+++ b/modelando los datos.xlsx
@@ -336,12 +336,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="T5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Usuario de Windows:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Arreglo de objetos con nuevos campos. 
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>MARCA</t>
   </si>
@@ -515,6 +540,9 @@
   </si>
   <si>
     <t>Info que se captura desde el backend</t>
+  </si>
+  <si>
+    <t>NUEVO CAMPOS</t>
   </si>
 </sst>
 </file>
@@ -634,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -673,12 +701,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,6 +709,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:W33"/>
+  <dimension ref="C3:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,53 +1022,56 @@
     <col min="14" max="14" width="13.42578125" customWidth="1"/>
     <col min="15" max="15" width="17.140625" customWidth="1"/>
     <col min="16" max="16" width="18.7109375" customWidth="1"/>
-    <col min="20" max="20" width="22.7109375" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" customWidth="1"/>
-    <col min="23" max="23" width="22.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" customWidth="1"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1"/>
+    <col min="24" max="24" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C3" s="17" t="s">
+    <row r="3" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="C3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-    </row>
-    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-    </row>
-    <row r="5" spans="3:23" ht="90" x14ac:dyDescent="0.25">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="17"/>
+    </row>
+    <row r="4" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="25"/>
+    </row>
+    <row r="5" spans="3:24" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1043,7 +1084,7 @@
       <c r="F5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="10" t="s">
@@ -1058,7 +1099,7 @@
       <c r="K5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="18" t="s">
         <v>45</v>
       </c>
       <c r="M5" s="7" t="s">
@@ -1067,35 +1108,38 @@
       <c r="N5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="Q5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="20" t="s">
+      <c r="R5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="S5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="V5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="V5" s="8" t="s">
+      <c r="W5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="W5" s="16" t="s">
+      <c r="X5" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1108,7 +1152,7 @@
       <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="19">
         <v>6</v>
       </c>
       <c r="H6" s="11" t="s">
@@ -1136,11 +1180,12 @@
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
-      <c r="S6" s="21" t="s">
+      <c r="S6" s="19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T6" s="26"/>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1158,8 +1203,9 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T7" s="27"/>
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1177,8 +1223,9 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T8" s="27"/>
+    </row>
+    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1196,8 +1243,9 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T9" s="27"/>
+    </row>
+    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1215,8 +1263,9 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T10" s="27"/>
+    </row>
+    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1234,8 +1283,9 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-    </row>
-    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T11" s="27"/>
+    </row>
+    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1253,8 +1303,9 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-    </row>
-    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T12" s="27"/>
+    </row>
+    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1272,8 +1323,9 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-    </row>
-    <row r="14" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T13" s="27"/>
+    </row>
+    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1291,8 +1343,9 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-    </row>
-    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T14" s="27"/>
+    </row>
+    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1310,8 +1363,9 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-    </row>
-    <row r="16" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T15" s="27"/>
+    </row>
+    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1329,8 +1383,9 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="27"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1348,8 +1403,9 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-    </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="27"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1367,8 +1423,9 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-    </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="27"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1386,8 +1443,9 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-    </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="27"/>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1405,8 +1463,9 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-    </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="27"/>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1424,8 +1483,9 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-    </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="27"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1443,8 +1503,9 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T22" s="27"/>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1462,8 +1523,9 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="27"/>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1481,8 +1543,9 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T24" s="27"/>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1500,8 +1563,9 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T25" s="27"/>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1519,8 +1583,9 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-    </row>
-    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T26" s="27"/>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1538,8 +1603,9 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
-    </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T27" s="27"/>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1557,8 +1623,9 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
-    </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T28" s="27"/>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1576,8 +1643,9 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
-    </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="T29" s="27"/>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1595,15 +1663,16 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
-    </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C32" s="22"/>
+      <c r="T30" s="27"/>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C32" s="20"/>
       <c r="D32" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="23"/>
+      <c r="C33" s="21"/>
       <c r="D33" t="s">
         <v>57</v>
       </c>
@@ -1634,27 +1703,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="D2" s="19" t="s">
+      <c r="B2" s="24"/>
+      <c r="D2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="K2" s="19" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="K2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="N2" s="19" t="s">
+      <c r="L2" s="24"/>
+      <c r="N2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="19"/>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">

</xml_diff>

<commit_message>
creacion de endpoint de consulta de inventario por id y se agrega campo de estado a diccionario inventario
</commit_message>
<xml_diff>
--- a/modelando los datos.xlsx
+++ b/modelando los datos.xlsx
@@ -328,11 +328,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-POR ASIGNAR
-ASIGNADO
-GARANTIA
-DADO DE BAJA
-MANTENIMIENTO</t>
+por asingar
+asignado
+garantia
+dado de baja
+mantenimiento</t>
         </r>
       </text>
     </comment>
@@ -709,6 +709,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,13 +725,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,46 +1030,46 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="22"/>
     </row>
     <row r="5" spans="3:24" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
@@ -1183,7 +1183,7 @@
       <c r="S6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="T6" s="26"/>
+      <c r="T6" s="23"/>
     </row>
     <row r="7" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
@@ -1203,7 +1203,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="27"/>
+      <c r="T7" s="24"/>
     </row>
     <row r="8" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
@@ -1223,7 +1223,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="27"/>
+      <c r="T8" s="24"/>
     </row>
     <row r="9" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
@@ -1243,7 +1243,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="27"/>
+      <c r="T9" s="24"/>
     </row>
     <row r="10" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
@@ -1263,7 +1263,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="27"/>
+      <c r="T10" s="24"/>
     </row>
     <row r="11" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
@@ -1283,7 +1283,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="27"/>
+      <c r="T11" s="24"/>
     </row>
     <row r="12" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
@@ -1303,7 +1303,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="27"/>
+      <c r="T12" s="24"/>
     </row>
     <row r="13" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
@@ -1323,7 +1323,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="27"/>
+      <c r="T13" s="24"/>
     </row>
     <row r="14" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
@@ -1343,7 +1343,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="27"/>
+      <c r="T14" s="24"/>
     </row>
     <row r="15" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
@@ -1363,7 +1363,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="27"/>
+      <c r="T15" s="24"/>
     </row>
     <row r="16" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
@@ -1383,7 +1383,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="27"/>
+      <c r="T16" s="24"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -1403,7 +1403,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="27"/>
+      <c r="T17" s="24"/>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
@@ -1423,7 +1423,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="27"/>
+      <c r="T18" s="24"/>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
@@ -1443,7 +1443,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="27"/>
+      <c r="T19" s="24"/>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
@@ -1463,7 +1463,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="27"/>
+      <c r="T20" s="24"/>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
@@ -1483,7 +1483,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="27"/>
+      <c r="T21" s="24"/>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
@@ -1503,7 +1503,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="27"/>
+      <c r="T22" s="24"/>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
@@ -1523,7 +1523,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="27"/>
+      <c r="T23" s="24"/>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
@@ -1543,7 +1543,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="27"/>
+      <c r="T24" s="24"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -1563,7 +1563,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="27"/>
+      <c r="T25" s="24"/>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
@@ -1583,7 +1583,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="27"/>
+      <c r="T26" s="24"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
@@ -1603,7 +1603,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
-      <c r="T27" s="27"/>
+      <c r="T27" s="24"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
@@ -1623,7 +1623,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
-      <c r="T28" s="27"/>
+      <c r="T28" s="24"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
@@ -1643,7 +1643,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
-      <c r="T29" s="27"/>
+      <c r="T29" s="24"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
@@ -1663,7 +1663,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
-      <c r="T30" s="27"/>
+      <c r="T30" s="24"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C32" s="20"/>
@@ -1703,27 +1703,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="D2" s="24" t="s">
+      <c r="B2" s="27"/>
+      <c r="D2" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="E2" s="27"/>
+      <c r="G2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="K2" s="24" t="s">
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="K2" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="N2" s="24" t="s">
+      <c r="L2" s="27"/>
+      <c r="N2" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="24"/>
+      <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">

</xml_diff>

<commit_message>
Creación endpoint traer registros de inventario por categoría y por usuario responsable
</commit_message>
<xml_diff>
--- a/modelando los datos.xlsx
+++ b/modelando los datos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HELMER\2021\gessys-servidor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HELMER\Proyectos\gessys-servidor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EBA38D-A81D-47D0-8325-73641124704B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,13 +26,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Usuario de Windows</author>
     <author>HELMER VILLARREAL</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -108,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -133,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -158,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -183,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -208,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -233,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="1" shapeId="0">
+    <comment ref="P5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -258,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0">
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -283,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0">
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -308,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S5" authorId="0" shapeId="0">
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -336,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T5" authorId="0" shapeId="0">
+    <comment ref="T5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -548,7 +549,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1004,11 +1005,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,7 +1689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>